<commit_message>
base timezone is us/pacific
(gets all matches on the same calendar day)
</commit_message>
<xml_diff>
--- a/tournaments/2026-mens-world-cup.xlsx
+++ b/tournaments/2026-mens-world-cup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/tournaments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1776D9-E38D-1749-AEA2-EC02B5A2DA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D16728-FEAB-7744-BA57-69AF23974B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="19740" activeTab="4" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="19740" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tournament" sheetId="8" r:id="rId1"/>
@@ -426,9 +426,6 @@
     <t>timezone</t>
   </si>
   <si>
-    <t>America/New_York</t>
-  </si>
-  <si>
     <t>WC 2026 Schedule / Scores</t>
   </si>
   <si>
@@ -1144,6 +1141,9 @@
   </si>
   <si>
     <t># source … https://hermann-baum.de/excel/WorldCup/en/</t>
+  </si>
+  <si>
+    <t>US/Pacific</t>
   </si>
 </sst>
 </file>
@@ -1152,7 +1152,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="166" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1234,14 +1234,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="166" formatCode="m/d/yy\ h:mm;@"/>
+      <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
@@ -1256,7 +1256,7 @@
       <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1296,14 +1296,14 @@
     <tableColumn id="1" xr3:uid="{35D3E9F5-BB3B-4940-9EB6-C927FD84875C}" name="match"/>
     <tableColumn id="2" xr3:uid="{97337EE3-AAC3-4452-8381-1A56C6B35138}" name="home-seed"/>
     <tableColumn id="3" xr3:uid="{AEDB8750-5B25-4357-9054-E49FECC94717}" name="away-seed"/>
-    <tableColumn id="4" xr3:uid="{B178F43D-E631-4314-9E59-2CDA6EDA94F1}" name="time" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{A42548B2-C8DF-4D47-B798-8E23FCB67696}" name="venue" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{B178F43D-E631-4314-9E59-2CDA6EDA94F1}" name="time" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{A42548B2-C8DF-4D47-B798-8E23FCB67696}" name="venue" dataDxfId="4"/>
     <tableColumn id="11" xr3:uid="{FC876643-4BF9-4FDA-A0ED-DF50FF384B1F}" name="home-team"/>
     <tableColumn id="10" xr3:uid="{E5D59926-7D0A-4689-A049-F55DB0E286E9}" name="away-team"/>
-    <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{967E27DF-151D-40C4-9623-59691A5D7311}" name="away-tiebreaker" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{967E27DF-151D-40C4-9623-59691A5D7311}" name="away-tiebreaker" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1641,11 +1641,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393FFACE-29F0-47F7-B7AD-389E0D6667C5}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1695,57 +1695,57 @@
         <v>76</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1753,28 +1753,28 @@
         <v>52</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1782,7 +1782,7 @@
         <v>127</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>128</v>
+        <v>367</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1797,28 +1797,28 @@
         <v>62</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1826,28 +1826,28 @@
         <v>63</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1855,28 +1855,28 @@
         <v>64</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1884,28 +1884,28 @@
         <v>65</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1913,28 +1913,28 @@
         <v>66</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1942,28 +1942,28 @@
         <v>67</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -2000,28 +2000,28 @@
         <v>69</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -2087,62 +2087,62 @@
         <v>93</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>97</v>
@@ -2171,65 +2171,65 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="H20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>108</v>
@@ -2596,10 +2596,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>226</v>
+      </c>
+      <c r="C18" t="s">
         <v>227</v>
-      </c>
-      <c r="C18" t="s">
-        <v>228</v>
       </c>
       <c r="D18" s="6">
         <v>46189.791666666664</v>
@@ -2613,10 +2613,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C19" t="s">
         <v>229</v>
-      </c>
-      <c r="C19" t="s">
-        <v>230</v>
       </c>
       <c r="D19" s="6">
         <v>46189.916666666664</v>
@@ -2630,10 +2630,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>230</v>
+      </c>
+      <c r="C20" t="s">
         <v>231</v>
-      </c>
-      <c r="C20" t="s">
-        <v>232</v>
       </c>
       <c r="D20" s="6">
         <v>46190.041666666664</v>
@@ -2647,10 +2647,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>232</v>
+      </c>
+      <c r="C21" t="s">
         <v>233</v>
-      </c>
-      <c r="C21" t="s">
-        <v>234</v>
       </c>
       <c r="D21" s="6">
         <v>46189.166666666664</v>
@@ -2664,10 +2664,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>240</v>
+      </c>
+      <c r="C22" t="s">
         <v>241</v>
-      </c>
-      <c r="C22" t="s">
-        <v>242</v>
       </c>
       <c r="D22" s="6">
         <v>46190.958333333328</v>
@@ -2681,10 +2681,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>238</v>
+      </c>
+      <c r="C23" t="s">
         <v>239</v>
-      </c>
-      <c r="C23" t="s">
-        <v>240</v>
       </c>
       <c r="D23" s="6">
         <v>46190.833333333328</v>
@@ -2698,10 +2698,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>234</v>
+      </c>
+      <c r="C24" t="s">
         <v>235</v>
-      </c>
-      <c r="C24" t="s">
-        <v>236</v>
       </c>
       <c r="D24" s="6">
         <v>46190.708333333328</v>
@@ -2715,10 +2715,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>236</v>
+      </c>
+      <c r="C25" t="s">
         <v>237</v>
-      </c>
-      <c r="C25" t="s">
-        <v>238</v>
       </c>
       <c r="D25" s="6">
         <v>46191.083333333328</v>
@@ -3004,10 +3004,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C42" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D42" s="6">
         <v>46196</v>
@@ -3021,10 +3021,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C43" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D43" s="6">
         <v>46195.875</v>
@@ -3038,10 +3038,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D44" s="6">
         <v>46195.708333333328</v>
@@ -3055,10 +3055,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C45" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D45" s="6">
         <v>46196.125</v>
@@ -3072,10 +3072,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D46" s="6">
         <v>46196.833333333328</v>
@@ -3089,10 +3089,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C47" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D47" s="6">
         <v>46196.958333333328</v>
@@ -3106,10 +3106,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C48" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D48" s="6">
         <v>46196.708333333328</v>
@@ -3123,10 +3123,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C49" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D49" s="6">
         <v>46197.083333333328</v>
@@ -3344,10 +3344,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C62" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D62" s="6">
         <v>46199.791666666664</v>
@@ -3361,10 +3361,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
+        <v>227</v>
+      </c>
+      <c r="C63" t="s">
         <v>228</v>
-      </c>
-      <c r="C63" t="s">
-        <v>229</v>
       </c>
       <c r="D63" s="6">
         <v>46199.791666666664</v>
@@ -3446,10 +3446,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C68" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D68" s="6">
         <v>46200.875</v>
@@ -3463,10 +3463,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
+        <v>239</v>
+      </c>
+      <c r="C69" t="s">
         <v>240</v>
-      </c>
-      <c r="C69" t="s">
-        <v>241</v>
       </c>
       <c r="D69" s="6">
         <v>46200.875</v>
@@ -3480,10 +3480,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
+        <v>231</v>
+      </c>
+      <c r="C70" t="s">
         <v>232</v>
-      </c>
-      <c r="C70" t="s">
-        <v>233</v>
       </c>
       <c r="D70" s="6">
         <v>46201.083333333328</v>
@@ -3497,10 +3497,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C71" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D71" s="6">
         <v>46201.083333333328</v>
@@ -3514,10 +3514,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C72" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D72" s="6">
         <v>46200.979166666664</v>
@@ -3531,10 +3531,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
+        <v>235</v>
+      </c>
+      <c r="C73" t="s">
         <v>236</v>
-      </c>
-      <c r="C73" t="s">
-        <v>237</v>
       </c>
       <c r="D73" s="6">
         <v>46200.979166666664</v>
@@ -3568,7 +3568,7 @@
         <v>40</v>
       </c>
       <c r="C75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D75" s="6">
         <v>46202.854166666664</v>
@@ -3616,10 +3616,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
+        <v>295</v>
+      </c>
+      <c r="C78" t="s">
         <v>296</v>
-      </c>
-      <c r="C78" t="s">
-        <v>297</v>
       </c>
       <c r="D78" s="6">
         <v>46203.875</v>
@@ -3636,7 +3636,7 @@
         <v>45</v>
       </c>
       <c r="C79" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D79" s="6">
         <v>46203.708333333328</v>
@@ -3653,7 +3653,7 @@
         <v>32</v>
       </c>
       <c r="C80" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D80" s="6">
         <v>46204.041666666664</v>
@@ -3667,10 +3667,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
+        <v>299</v>
+      </c>
+      <c r="C81" t="s">
         <v>300</v>
-      </c>
-      <c r="C81" t="s">
-        <v>301</v>
       </c>
       <c r="D81" s="6">
         <v>46204.666666666664</v>
@@ -3687,7 +3687,7 @@
         <v>38</v>
       </c>
       <c r="C82" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D82" s="6">
         <v>46205</v>
@@ -3704,7 +3704,7 @@
         <v>42</v>
       </c>
       <c r="C83" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D83" s="6">
         <v>46204.833333333328</v>
@@ -3718,10 +3718,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
+        <v>303</v>
+      </c>
+      <c r="C84" t="s">
         <v>304</v>
-      </c>
-      <c r="C84" t="s">
-        <v>305</v>
       </c>
       <c r="D84" s="6">
         <v>46205.958333333328</v>
@@ -3738,7 +3738,7 @@
         <v>46</v>
       </c>
       <c r="C85" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D85" s="6">
         <v>46205.791666666664</v>
@@ -3755,7 +3755,7 @@
         <v>36</v>
       </c>
       <c r="C86" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D86" s="6">
         <v>46206.125</v>
@@ -3769,7 +3769,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C87" t="s">
         <v>43</v>
@@ -3786,10 +3786,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
+        <v>308</v>
+      </c>
+      <c r="C88" t="s">
         <v>309</v>
-      </c>
-      <c r="C88" t="s">
-        <v>310</v>
       </c>
       <c r="D88" s="6">
         <v>46207.0625</v>
@@ -3820,10 +3820,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
+        <v>310</v>
+      </c>
+      <c r="C90" t="s">
         <v>311</v>
-      </c>
-      <c r="C90" t="s">
-        <v>312</v>
       </c>
       <c r="D90" s="6">
         <v>46207.875</v>
@@ -3837,10 +3837,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
+        <v>312</v>
+      </c>
+      <c r="C91" t="s">
         <v>313</v>
-      </c>
-      <c r="C91" t="s">
-        <v>314</v>
       </c>
       <c r="D91" s="6">
         <v>46207.708333333328</v>
@@ -3854,10 +3854,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
+        <v>314</v>
+      </c>
+      <c r="C92" t="s">
         <v>315</v>
-      </c>
-      <c r="C92" t="s">
-        <v>316</v>
       </c>
       <c r="D92" s="6">
         <v>46208.833333333328</v>
@@ -3871,10 +3871,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
+        <v>316</v>
+      </c>
+      <c r="C93" t="s">
         <v>317</v>
-      </c>
-      <c r="C93" t="s">
-        <v>318</v>
       </c>
       <c r="D93" s="6">
         <v>46209</v>
@@ -3888,10 +3888,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
+        <v>318</v>
+      </c>
+      <c r="C94" t="s">
         <v>319</v>
-      </c>
-      <c r="C94" t="s">
-        <v>320</v>
       </c>
       <c r="D94" s="6">
         <v>46209.791666666664</v>
@@ -3905,10 +3905,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
+        <v>320</v>
+      </c>
+      <c r="C95" t="s">
         <v>321</v>
-      </c>
-      <c r="C95" t="s">
-        <v>322</v>
       </c>
       <c r="D95" s="6">
         <v>46210</v>
@@ -3922,10 +3922,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
+        <v>322</v>
+      </c>
+      <c r="C96" t="s">
         <v>323</v>
-      </c>
-      <c r="C96" t="s">
-        <v>324</v>
       </c>
       <c r="D96" s="6">
         <v>46210.666666666664</v>
@@ -3939,10 +3939,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
+        <v>324</v>
+      </c>
+      <c r="C97" t="s">
         <v>325</v>
-      </c>
-      <c r="C97" t="s">
-        <v>326</v>
       </c>
       <c r="D97" s="6">
         <v>46210.833333333328</v>
@@ -3956,10 +3956,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
+        <v>326</v>
+      </c>
+      <c r="C98" t="s">
         <v>327</v>
-      </c>
-      <c r="C98" t="s">
-        <v>328</v>
       </c>
       <c r="D98" s="6">
         <v>46212.833333333328</v>
@@ -3973,10 +3973,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
+        <v>328</v>
+      </c>
+      <c r="C99" t="s">
         <v>329</v>
-      </c>
-      <c r="C99" t="s">
-        <v>330</v>
       </c>
       <c r="D99" s="6">
         <v>46213.791666666664</v>
@@ -3990,10 +3990,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
+        <v>330</v>
+      </c>
+      <c r="C100" t="s">
         <v>331</v>
-      </c>
-      <c r="C100" t="s">
-        <v>332</v>
       </c>
       <c r="D100" s="6">
         <v>46214.875</v>
@@ -4007,10 +4007,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
+        <v>332</v>
+      </c>
+      <c r="C101" t="s">
         <v>333</v>
-      </c>
-      <c r="C101" t="s">
-        <v>334</v>
       </c>
       <c r="D101" s="6">
         <v>46215.041666666664</v>
@@ -4024,10 +4024,10 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
+        <v>334</v>
+      </c>
+      <c r="C102" t="s">
         <v>335</v>
-      </c>
-      <c r="C102" t="s">
-        <v>336</v>
       </c>
       <c r="D102" s="6">
         <v>46217.791666666664</v>
@@ -4041,10 +4041,10 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
+        <v>336</v>
+      </c>
+      <c r="C103" t="s">
         <v>337</v>
-      </c>
-      <c r="C103" t="s">
-        <v>338</v>
       </c>
       <c r="D103" s="6">
         <v>46218.791666666664</v>
@@ -4058,10 +4058,10 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
+        <v>359</v>
+      </c>
+      <c r="C104" t="s">
         <v>360</v>
-      </c>
-      <c r="C104" t="s">
-        <v>361</v>
       </c>
       <c r="D104" s="6">
         <v>46221.875</v>
@@ -4075,10 +4075,10 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
+        <v>338</v>
+      </c>
+      <c r="C105" t="s">
         <v>339</v>
-      </c>
-      <c r="C105" t="s">
-        <v>340</v>
       </c>
       <c r="D105" s="6">
         <v>46222.791666666664</v>
@@ -4120,7 +4120,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -4128,7 +4128,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -4136,7 +4136,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -4144,7 +4144,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -4152,7 +4152,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -4160,7 +4160,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -4168,7 +4168,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -4176,7 +4176,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -4184,7 +4184,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -4192,7 +4192,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -4200,7 +4200,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -4208,7 +4208,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -4224,7 +4224,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -4232,7 +4232,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -4240,7 +4240,7 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -4248,7 +4248,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -4256,7 +4256,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -4264,7 +4264,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -4272,7 +4272,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -4280,7 +4280,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -4288,7 +4288,7 @@
         <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -4296,7 +4296,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -4304,7 +4304,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -4312,7 +4312,7 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -4320,7 +4320,7 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -4328,7 +4328,7 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -4336,7 +4336,7 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -4344,7 +4344,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -4352,7 +4352,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -4360,7 +4360,7 @@
         <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -4368,76 +4368,76 @@
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B36" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B37" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B39" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B40" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B41" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B42" t="s">
         <v>54</v>
@@ -4445,58 +4445,58 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B43" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B44" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B45" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B47" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B48" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B49" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -4513,7 +4513,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4555,7 +4555,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>111</v>
@@ -4610,7 +4610,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B7" t="s">
         <v>125</v>
@@ -4632,7 +4632,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B9" t="s">
         <v>123</v>
@@ -4643,24 +4643,24 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B10" t="s">
+        <v>287</v>
+      </c>
+      <c r="J10" t="s">
         <v>288</v>
-      </c>
-      <c r="J10" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B11" t="s">
+        <v>289</v>
+      </c>
+      <c r="J11" t="s">
         <v>290</v>
-      </c>
-      <c r="J11" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -4668,153 +4668,153 @@
         <v>91</v>
       </c>
       <c r="B12" t="s">
+        <v>275</v>
+      </c>
+      <c r="J12" t="s">
         <v>276</v>
-      </c>
-      <c r="J12" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B13" t="s">
+        <v>292</v>
+      </c>
+      <c r="J13" t="s">
         <v>293</v>
-      </c>
-      <c r="J13" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B16" t="s">
+        <v>255</v>
+      </c>
+      <c r="J16" t="s">
         <v>256</v>
-      </c>
-      <c r="J16" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B18" t="s">
+        <v>272</v>
+      </c>
+      <c r="J18" t="s">
         <v>273</v>
-      </c>
-      <c r="J18" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B20" t="s">
+        <v>275</v>
+      </c>
+      <c r="J20" t="s">
         <v>276</v>
-      </c>
-      <c r="J20" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B21" t="s">
+        <v>277</v>
+      </c>
+      <c r="J21" t="s">
         <v>278</v>
-      </c>
-      <c r="J21" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B22" t="s">
+        <v>279</v>
+      </c>
+      <c r="J22" t="s">
         <v>280</v>
-      </c>
-      <c r="J22" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B23" t="s">
+        <v>281</v>
+      </c>
+      <c r="J23" t="s">
         <v>282</v>
-      </c>
-      <c r="J23" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B24" t="s">
+        <v>283</v>
+      </c>
+      <c r="J24" t="s">
         <v>284</v>
-      </c>
-      <c r="J24" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B25" t="s">
+        <v>285</v>
+      </c>
+      <c r="J25" t="s">
         <v>286</v>
-      </c>
-      <c r="J25" t="s">
-        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -4830,7 +4830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E21D59-11F2-6647-B74E-6B03465C0273}">
   <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -4841,22 +4841,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1" t="s">
         <v>362</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>363</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>364</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>365</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>366</v>
-      </c>
-      <c r="F1" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -5136,10 +5136,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>226</v>
+      </c>
+      <c r="C18" t="s">
         <v>227</v>
-      </c>
-      <c r="C18" t="s">
-        <v>228</v>
       </c>
       <c r="D18" s="6">
         <v>46189.791666666664</v>
@@ -5153,10 +5153,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C19" t="s">
         <v>229</v>
-      </c>
-      <c r="C19" t="s">
-        <v>230</v>
       </c>
       <c r="D19" s="6">
         <v>46189.916666666664</v>
@@ -5170,10 +5170,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>230</v>
+      </c>
+      <c r="C20" t="s">
         <v>231</v>
-      </c>
-      <c r="C20" t="s">
-        <v>232</v>
       </c>
       <c r="D20" s="6">
         <v>46190.041666666664</v>
@@ -5187,10 +5187,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>232</v>
+      </c>
+      <c r="C21" t="s">
         <v>233</v>
-      </c>
-      <c r="C21" t="s">
-        <v>234</v>
       </c>
       <c r="D21" s="6">
         <v>46189.166666666664</v>
@@ -5204,10 +5204,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>240</v>
+      </c>
+      <c r="C22" t="s">
         <v>241</v>
-      </c>
-      <c r="C22" t="s">
-        <v>242</v>
       </c>
       <c r="D22" s="6">
         <v>46190.958333333328</v>
@@ -5221,10 +5221,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>238</v>
+      </c>
+      <c r="C23" t="s">
         <v>239</v>
-      </c>
-      <c r="C23" t="s">
-        <v>240</v>
       </c>
       <c r="D23" s="6">
         <v>46190.833333333328</v>
@@ -5238,10 +5238,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>234</v>
+      </c>
+      <c r="C24" t="s">
         <v>235</v>
-      </c>
-      <c r="C24" t="s">
-        <v>236</v>
       </c>
       <c r="D24" s="6">
         <v>46190.708333333328</v>
@@ -5255,10 +5255,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>236</v>
+      </c>
+      <c r="C25" t="s">
         <v>237</v>
-      </c>
-      <c r="C25" t="s">
-        <v>238</v>
       </c>
       <c r="D25" s="6">
         <v>46191.083333333328</v>
@@ -5544,10 +5544,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C42" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D42" s="6">
         <v>46196</v>
@@ -5561,10 +5561,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C43" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D43" s="6">
         <v>46195.875</v>
@@ -5578,10 +5578,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D44" s="6">
         <v>46195.708333333328</v>
@@ -5595,10 +5595,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C45" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D45" s="6">
         <v>46196.125</v>
@@ -5612,10 +5612,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D46" s="6">
         <v>46196.833333333328</v>
@@ -5629,10 +5629,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C47" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D47" s="6">
         <v>46196.958333333328</v>
@@ -5646,10 +5646,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C48" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D48" s="6">
         <v>46196.708333333328</v>
@@ -5663,10 +5663,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C49" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D49" s="6">
         <v>46197.083333333328</v>
@@ -5884,10 +5884,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C62" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D62" s="6">
         <v>46199.791666666664</v>
@@ -5901,10 +5901,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
+        <v>227</v>
+      </c>
+      <c r="C63" t="s">
         <v>228</v>
-      </c>
-      <c r="C63" t="s">
-        <v>229</v>
       </c>
       <c r="D63" s="6">
         <v>46199.791666666664</v>
@@ -5986,10 +5986,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C68" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D68" s="6">
         <v>46200.875</v>
@@ -6003,10 +6003,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
+        <v>239</v>
+      </c>
+      <c r="C69" t="s">
         <v>240</v>
-      </c>
-      <c r="C69" t="s">
-        <v>241</v>
       </c>
       <c r="D69" s="6">
         <v>46200.875</v>
@@ -6020,10 +6020,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
+        <v>231</v>
+      </c>
+      <c r="C70" t="s">
         <v>232</v>
-      </c>
-      <c r="C70" t="s">
-        <v>233</v>
       </c>
       <c r="D70" s="6">
         <v>46201.083333333328</v>
@@ -6037,10 +6037,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C71" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D71" s="6">
         <v>46201.083333333328</v>
@@ -6054,10 +6054,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C72" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D72" s="6">
         <v>46200.979166666664</v>
@@ -6071,10 +6071,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
+        <v>235</v>
+      </c>
+      <c r="C73" t="s">
         <v>236</v>
-      </c>
-      <c r="C73" t="s">
-        <v>237</v>
       </c>
       <c r="D73" s="6">
         <v>46200.979166666664</v>
@@ -6108,7 +6108,7 @@
         <v>40</v>
       </c>
       <c r="C75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D75" s="6">
         <v>46202.854166666664</v>
@@ -6156,10 +6156,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
+        <v>295</v>
+      </c>
+      <c r="C78" t="s">
         <v>296</v>
-      </c>
-      <c r="C78" t="s">
-        <v>297</v>
       </c>
       <c r="D78" s="6">
         <v>46203.875</v>
@@ -6176,7 +6176,7 @@
         <v>45</v>
       </c>
       <c r="C79" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D79" s="6">
         <v>46203.708333333328</v>
@@ -6193,7 +6193,7 @@
         <v>32</v>
       </c>
       <c r="C80" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D80" s="6">
         <v>46204.041666666664</v>
@@ -6207,10 +6207,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
+        <v>299</v>
+      </c>
+      <c r="C81" t="s">
         <v>300</v>
-      </c>
-      <c r="C81" t="s">
-        <v>301</v>
       </c>
       <c r="D81" s="6">
         <v>46204.666666666664</v>
@@ -6227,7 +6227,7 @@
         <v>38</v>
       </c>
       <c r="C82" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D82" s="6">
         <v>46205</v>
@@ -6244,7 +6244,7 @@
         <v>42</v>
       </c>
       <c r="C83" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D83" s="6">
         <v>46204.833333333328</v>
@@ -6258,10 +6258,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
+        <v>303</v>
+      </c>
+      <c r="C84" t="s">
         <v>304</v>
-      </c>
-      <c r="C84" t="s">
-        <v>305</v>
       </c>
       <c r="D84" s="6">
         <v>46205.958333333328</v>
@@ -6278,7 +6278,7 @@
         <v>46</v>
       </c>
       <c r="C85" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D85" s="6">
         <v>46205.791666666664</v>
@@ -6295,7 +6295,7 @@
         <v>36</v>
       </c>
       <c r="C86" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D86" s="6">
         <v>46206.125</v>
@@ -6309,7 +6309,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C87" t="s">
         <v>43</v>
@@ -6326,10 +6326,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
+        <v>308</v>
+      </c>
+      <c r="C88" t="s">
         <v>309</v>
-      </c>
-      <c r="C88" t="s">
-        <v>310</v>
       </c>
       <c r="D88" s="6">
         <v>46207.0625</v>
@@ -6360,10 +6360,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
+        <v>310</v>
+      </c>
+      <c r="C90" t="s">
         <v>311</v>
-      </c>
-      <c r="C90" t="s">
-        <v>312</v>
       </c>
       <c r="D90" s="6">
         <v>46207.875</v>
@@ -6377,10 +6377,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
+        <v>312</v>
+      </c>
+      <c r="C91" t="s">
         <v>313</v>
-      </c>
-      <c r="C91" t="s">
-        <v>314</v>
       </c>
       <c r="D91" s="6">
         <v>46207.708333333328</v>
@@ -6394,10 +6394,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
+        <v>314</v>
+      </c>
+      <c r="C92" t="s">
         <v>315</v>
-      </c>
-      <c r="C92" t="s">
-        <v>316</v>
       </c>
       <c r="D92" s="6">
         <v>46208.833333333328</v>
@@ -6411,10 +6411,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
+        <v>316</v>
+      </c>
+      <c r="C93" t="s">
         <v>317</v>
-      </c>
-      <c r="C93" t="s">
-        <v>318</v>
       </c>
       <c r="D93" s="6">
         <v>46209</v>
@@ -6428,10 +6428,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
+        <v>318</v>
+      </c>
+      <c r="C94" t="s">
         <v>319</v>
-      </c>
-      <c r="C94" t="s">
-        <v>320</v>
       </c>
       <c r="D94" s="6">
         <v>46209.791666666664</v>
@@ -6445,10 +6445,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
+        <v>320</v>
+      </c>
+      <c r="C95" t="s">
         <v>321</v>
-      </c>
-      <c r="C95" t="s">
-        <v>322</v>
       </c>
       <c r="D95" s="6">
         <v>46210</v>
@@ -6462,10 +6462,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
+        <v>322</v>
+      </c>
+      <c r="C96" t="s">
         <v>323</v>
-      </c>
-      <c r="C96" t="s">
-        <v>324</v>
       </c>
       <c r="D96" s="6">
         <v>46210.666666666664</v>
@@ -6479,10 +6479,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
+        <v>324</v>
+      </c>
+      <c r="C97" t="s">
         <v>325</v>
-      </c>
-      <c r="C97" t="s">
-        <v>326</v>
       </c>
       <c r="D97" s="6">
         <v>46210.833333333328</v>
@@ -6496,10 +6496,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
+        <v>326</v>
+      </c>
+      <c r="C98" t="s">
         <v>327</v>
-      </c>
-      <c r="C98" t="s">
-        <v>328</v>
       </c>
       <c r="D98" s="6">
         <v>46212.833333333328</v>
@@ -6513,10 +6513,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
+        <v>328</v>
+      </c>
+      <c r="C99" t="s">
         <v>329</v>
-      </c>
-      <c r="C99" t="s">
-        <v>330</v>
       </c>
       <c r="D99" s="6">
         <v>46213.791666666664</v>
@@ -6530,10 +6530,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
+        <v>330</v>
+      </c>
+      <c r="C100" t="s">
         <v>331</v>
-      </c>
-      <c r="C100" t="s">
-        <v>332</v>
       </c>
       <c r="D100" s="6">
         <v>46214.875</v>
@@ -6547,10 +6547,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
+        <v>332</v>
+      </c>
+      <c r="C101" t="s">
         <v>333</v>
-      </c>
-      <c r="C101" t="s">
-        <v>334</v>
       </c>
       <c r="D101" s="6">
         <v>46215.041666666664</v>
@@ -6564,10 +6564,10 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
+        <v>334</v>
+      </c>
+      <c r="C102" t="s">
         <v>335</v>
-      </c>
-      <c r="C102" t="s">
-        <v>336</v>
       </c>
       <c r="D102" s="6">
         <v>46217.791666666664</v>
@@ -6581,10 +6581,10 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
+        <v>336</v>
+      </c>
+      <c r="C103" t="s">
         <v>337</v>
-      </c>
-      <c r="C103" t="s">
-        <v>338</v>
       </c>
       <c r="D103" s="6">
         <v>46218.791666666664</v>
@@ -6598,10 +6598,10 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
+        <v>359</v>
+      </c>
+      <c r="C104" t="s">
         <v>360</v>
-      </c>
-      <c r="C104" t="s">
-        <v>361</v>
       </c>
       <c r="D104" s="6">
         <v>46221.875</v>
@@ -6615,10 +6615,10 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
+        <v>338</v>
+      </c>
+      <c r="C105" t="s">
         <v>339</v>
-      </c>
-      <c r="C105" t="s">
-        <v>340</v>
       </c>
       <c r="D105" s="6">
         <v>46222.791666666664</v>

</xml_diff>